<commit_message>
(fix) reporting: sizing file
</commit_message>
<xml_diff>
--- a/en/assets/reporting/installation/Centreon-MBI-QuickGuide-Storage-Sizing_EN.xlsx
+++ b/en/assets/reporting/installation/Centreon-MBI-QuickGuide-Storage-Sizing_EN.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28502"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennegautier/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\centreon-documentation\en\assets\reporting\installation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85485104-71CF-4631-9126-4D4E666944D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="-21040" windowWidth="33600" windowHeight="20460" tabRatio="289"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="289" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server storage sizing" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -153,7 +162,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
@@ -378,7 +387,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Milliers" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -392,6 +401,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -414,7 +426,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1"/>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -817,39 +835,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="19.1640625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="12.1640625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="24.5" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="24.42578125" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -859,7 +877,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -869,7 +887,7 @@
       </c>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="19" t="s">
         <v>32</v>
       </c>
@@ -883,7 +901,7 @@
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -891,7 +909,7 @@
       <c r="J6" s="3"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
@@ -905,7 +923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -919,7 +937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -933,7 +951,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -947,7 +965,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -959,7 +977,7 @@
       <c r="I11" s="12"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -971,7 +989,7 @@
       <c r="I12" s="12"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -983,7 +1001,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>29</v>
       </c>
@@ -995,7 +1013,7 @@
       <c r="I14" s="11"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>30</v>
       </c>
@@ -1003,7 +1021,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -1011,7 +1029,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -1019,18 +1037,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F18" s="18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E19" s="15"/>
       <c r="F19" s="20">
         <v>2.8</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>17</v>
       </c>
@@ -1052,7 +1070,7 @@
       <c r="H20" s="7"/>
       <c r="I20" s="8"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>35</v>
       </c>
@@ -1061,14 +1079,14 @@
       </c>
       <c r="C21" s="13">
         <f>((E21*D21)*2)/1024/1024</f>
-        <v>13842.7734375</v>
+        <v>98876.953125</v>
       </c>
       <c r="D21" s="20">
         <f>(60/$B$17)*24*B21*$B$9*$B$16</f>
         <v>518400000</v>
       </c>
       <c r="E21" s="20">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="F21" s="20" t="s">
         <v>28</v>
@@ -1076,7 +1094,7 @@
       <c r="H21" s="7"/>
       <c r="I21" s="8"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>37</v>
       </c>
@@ -1101,7 +1119,7 @@
       <c r="H22" s="7"/>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>38</v>
       </c>
@@ -1126,7 +1144,7 @@
       <c r="H23" s="7"/>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>36</v>
       </c>
@@ -1151,7 +1169,7 @@
       <c r="H24" s="7"/>
       <c r="I24" s="8"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>39</v>
       </c>
@@ -1168,7 +1186,7 @@
       <c r="H25" s="7"/>
       <c r="I25" s="8"/>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>20</v>
       </c>
@@ -1194,7 +1212,7 @@
       <c r="H26" s="7"/>
       <c r="I26" s="8"/>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
         <v>21</v>
       </c>
@@ -1220,7 +1238,7 @@
       <c r="H27" s="7"/>
       <c r="I27" s="8"/>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
         <v>18</v>
       </c>
@@ -1246,7 +1264,7 @@
       <c r="H28" s="7"/>
       <c r="I28" s="8"/>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>19</v>
       </c>
@@ -1272,14 +1290,14 @@
       <c r="H29" s="7"/>
       <c r="I29" s="8"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="23"/>
       <c r="B30" s="23" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="14">
         <f>SUM(C21:C25)</f>
-        <v>109674.44266042401</v>
+        <v>194708.62234792401</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="8"/>

</xml_diff>